<commit_message>
👨‍💻 Actualizando visualización reportes
</commit_message>
<xml_diff>
--- a/vistas/modulos/Reporte_Contratados.xlsx
+++ b/vistas/modulos/Reporte_Contratados.xlsx
@@ -142,7 +142,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -654,12 +654,12 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>0017</t>
+          <t>0002</t>
         </is>
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t>RESIDENCIAL LAS PILETAS</t>
+          <t>GERENCIA ADMINISTRATIVA</t>
         </is>
       </c>
     </row>
@@ -765,6 +765,774 @@
         </is>
       </c>
       <c r="U9" s="5" t="inlineStr">
+        <is>
+          <t>MOTIVO</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>003348</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>ROBERTO   HERNANDEZ LOPEZ/SIN UNIFORME</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>250.00 </t>
+        </is>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="F10" s="1" t="inlineStr">
+        <is>
+          <t>2025-03-03 00:00:00 </t>
+        </is>
+      </c>
+      <c r="G10" s="1" t="inlineStr">
+        <is>
+          <t>2030-11-20 00:00:00  </t>
+        </is>
+      </c>
+      <c r="H10" s="1" t="inlineStr">
+        <is>
+          <t>F.RETIRO</t>
+        </is>
+      </c>
+      <c r="I10" s="1" t="inlineStr">
+        <is>
+          <t>******</t>
+        </is>
+      </c>
+      <c r="J10" s="1" t="inlineStr">
+        <is>
+          <t>31/03/04</t>
+        </is>
+      </c>
+      <c r="K10" s="1" t="inlineStr">
+        <is>
+          <t>02031000-1</t>
+        </is>
+      </c>
+      <c r="L10" s="1" t="inlineStr">
+        <is>
+          <t>68871345</t>
+        </is>
+      </c>
+      <c r="M10" s="1" t="inlineStr">
+        <is>
+          <t>0003</t>
+        </is>
+      </c>
+      <c r="N10" s="1" t="inlineStr">
+        <is>
+          <t>GUARDAESPALDA</t>
+        </is>
+      </c>
+      <c r="O10" s="1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="P10" s="1" t="inlineStr">
+        <is>
+          <t>0000-00-00</t>
+        </is>
+      </c>
+      <c r="Q10" s="1" t="inlineStr">
+        <is>
+          <t>199680452</t>
+        </is>
+      </c>
+      <c r="R10" s="1" t="inlineStr">
+        <is>
+          <t>0614 180868 112 3</t>
+        </is>
+      </c>
+      <c r="S10" s="1" t="inlineStr">
+        <is>
+          <t>0368-052358-4</t>
+        </is>
+      </c>
+      <c r="T10" s="1" t="inlineStr">
+        <is>
+          <t>MOTIVO</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>002258</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>CELIA NOEMI  BARILLAS ZEPEDA/SIN UNIFORME</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>0.00 </t>
+        </is>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="F11" s="1" t="inlineStr">
+        <is>
+          <t>0000-00-00 00:00:00 </t>
+        </is>
+      </c>
+      <c r="G11" s="1" t="inlineStr">
+        <is>
+          <t>2014-08-16 00:00:00  </t>
+        </is>
+      </c>
+      <c r="H11" s="1" t="inlineStr">
+        <is>
+          <t>F.RETIRO</t>
+        </is>
+      </c>
+      <c r="I11" s="1" t="inlineStr">
+        <is>
+          <t>******</t>
+        </is>
+      </c>
+      <c r="J11" s="1" t="inlineStr">
+        <is>
+          <t>00575460-4</t>
+        </is>
+      </c>
+      <c r="K11" s="1" t="inlineStr">
+        <is>
+          <t>269697160000</t>
+        </is>
+      </c>
+      <c r="L11" s="1" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="M11" s="1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="N11" s="1" t="inlineStr">
+        <is>
+          <t>0000-00-00</t>
+        </is>
+      </c>
+      <c r="O11" s="1" t="inlineStr">
+        <is>
+          <t>193732558</t>
+        </is>
+      </c>
+      <c r="P11" s="1" t="inlineStr">
+        <is>
+          <t>0816-031173-101-3</t>
+        </is>
+      </c>
+      <c r="Q11" s="1" t="inlineStr">
+        <is>
+          <t>0122-038904-1</t>
+        </is>
+      </c>
+      <c r="R11" s="1" t="inlineStr">
+        <is>
+          <t>MOTIVO</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>010593</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>ELIZABETH DEL CARMEN  RECINOS HERNANDEZ/SIN UNIFORME</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>0.00 </t>
+        </is>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="F12" s="1" t="inlineStr">
+        <is>
+          <t>2006-01-15 00:00:00 </t>
+        </is>
+      </c>
+      <c r="G12" s="1" t="inlineStr">
+        <is>
+          <t>2006-01-20 00:00:00  </t>
+        </is>
+      </c>
+      <c r="H12" s="1" t="inlineStr">
+        <is>
+          <t>F.RETIRO</t>
+        </is>
+      </c>
+      <c r="I12" s="1" t="inlineStr">
+        <is>
+          <t>******</t>
+        </is>
+      </c>
+      <c r="J12" s="1" t="inlineStr">
+        <is>
+          <t>07/01/15</t>
+        </is>
+      </c>
+      <c r="K12" s="1" t="inlineStr">
+        <is>
+          <t>02250350-3</t>
+        </is>
+      </c>
+      <c r="L12" s="1" t="inlineStr">
+        <is>
+          <t>255127080005</t>
+        </is>
+      </c>
+      <c r="M12" s="1" t="inlineStr">
+        <is>
+          <t>0001</t>
+        </is>
+      </c>
+      <c r="N12" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE ADMINISTRATIVO</t>
+        </is>
+      </c>
+      <c r="O12" s="1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="P12" s="1" t="inlineStr">
+        <is>
+          <t>0000-00-00</t>
+        </is>
+      </c>
+      <c r="Q12" s="1" t="inlineStr">
+        <is>
+          <t>389694555</t>
+        </is>
+      </c>
+      <c r="R12" s="1" t="inlineStr">
+        <is>
+          <t>0614-071169-110-1</t>
+        </is>
+      </c>
+      <c r="S12" s="1" t="inlineStr">
+        <is>
+          <t>0322-045110-3</t>
+        </is>
+      </c>
+      <c r="T12" s="1" t="inlineStr">
+        <is>
+          <t>MOTIVO</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>011988</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>LUIS FRANCISCO  RECINOS HENRIQUEZ/SIN UNIFORME</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>0.00 </t>
+        </is>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="F13" s="1" t="inlineStr">
+        <is>
+          <t>2001-11-17 00:00:00 </t>
+        </is>
+      </c>
+      <c r="G13" s="1" t="inlineStr">
+        <is>
+          <t>2001-11-17 00:00:00  </t>
+        </is>
+      </c>
+      <c r="H13" s="1" t="inlineStr">
+        <is>
+          <t>F.RETIRO</t>
+        </is>
+      </c>
+      <c r="I13" s="1" t="inlineStr">
+        <is>
+          <t>******</t>
+        </is>
+      </c>
+      <c r="J13" s="1" t="inlineStr">
+        <is>
+          <t>05010802-8</t>
+        </is>
+      </c>
+      <c r="K13" s="1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L13" s="1" t="inlineStr">
+        <is>
+          <t>0000</t>
+        </is>
+      </c>
+      <c r="M13" s="1" t="inlineStr">
+        <is>
+          <t>MANTENIMIENTO</t>
+        </is>
+      </c>
+      <c r="N13" s="1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="O13" s="1" t="inlineStr">
+        <is>
+          <t>0000-00-00</t>
+        </is>
+      </c>
+      <c r="P13" s="1" t="inlineStr">
+        <is>
+          <t>0302-300694-101-0</t>
+        </is>
+      </c>
+      <c r="Q13" s="1" t="inlineStr">
+        <is>
+          <t>0366-043123-5</t>
+        </is>
+      </c>
+      <c r="R13" s="1" t="inlineStr">
+        <is>
+          <t>MOTIVO</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>013203</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>JOSE BENJAMIN  SANTOS HERNANDEZ/SIN UNIFORME</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>305.00 </t>
+        </is>
+      </c>
+      <c r="D14" s="1" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E14" s="1" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="F14" s="1" t="inlineStr">
+        <is>
+          <t>2017-10-19 00:00:00 </t>
+        </is>
+      </c>
+      <c r="G14" s="1" t="inlineStr">
+        <is>
+          <t>2017-10-19 00:00:00  </t>
+        </is>
+      </c>
+      <c r="H14" s="1" t="inlineStr">
+        <is>
+          <t>F.RETIRO</t>
+        </is>
+      </c>
+      <c r="I14" s="1" t="inlineStr">
+        <is>
+          <t>******</t>
+        </is>
+      </c>
+      <c r="J14" s="1" t="inlineStr">
+        <is>
+          <t>17/10/19</t>
+        </is>
+      </c>
+      <c r="K14" s="1" t="inlineStr">
+        <is>
+          <t>02264938-3</t>
+        </is>
+      </c>
+      <c r="L14" s="1" t="inlineStr">
+        <is>
+          <t>275402640001</t>
+        </is>
+      </c>
+      <c r="M14" s="1" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="N14" s="1" t="inlineStr">
+        <is>
+          <t>AGENTE DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="O14" s="1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="P14" s="1" t="inlineStr">
+        <is>
+          <t>0000-00-00</t>
+        </is>
+      </c>
+      <c r="Q14" s="1" t="inlineStr">
+        <is>
+          <t>106750779</t>
+        </is>
+      </c>
+      <c r="R14" s="1" t="inlineStr">
+        <is>
+          <t>0210-280575-110-4</t>
+        </is>
+      </c>
+      <c r="S14" s="1" t="inlineStr">
+        <is>
+          <t>0311-109439-1</t>
+        </is>
+      </c>
+      <c r="T14" s="1" t="inlineStr">
+        <is>
+          <t>MOTIVO</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>013882</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>HUGO LUIS  BARILLAS SANABRIA/SIN UNIFORME</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>305.00 </t>
+        </is>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="F15" s="1" t="inlineStr">
+        <is>
+          <t>2021-01-21 00:00:00 </t>
+        </is>
+      </c>
+      <c r="G15" s="1" t="inlineStr">
+        <is>
+          <t>2021-01-21 00:00:00  </t>
+        </is>
+      </c>
+      <c r="H15" s="1" t="inlineStr">
+        <is>
+          <t>F.RETIRO</t>
+        </is>
+      </c>
+      <c r="I15" s="1" t="inlineStr">
+        <is>
+          <t>******</t>
+        </is>
+      </c>
+      <c r="J15" s="1" t="inlineStr">
+        <is>
+          <t>26/01/21</t>
+        </is>
+      </c>
+      <c r="K15" s="1" t="inlineStr">
+        <is>
+          <t>03356690-4</t>
+        </is>
+      </c>
+      <c r="L15" s="1" t="inlineStr">
+        <is>
+          <t>313512220018</t>
+        </is>
+      </c>
+      <c r="M15" s="1" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="N15" s="1" t="inlineStr">
+        <is>
+          <t>AGENTE DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="O15" s="1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="P15" s="1" t="inlineStr">
+        <is>
+          <t>0000-00-00</t>
+        </is>
+      </c>
+      <c r="Q15" s="1" t="inlineStr">
+        <is>
+          <t>106856963</t>
+        </is>
+      </c>
+      <c r="R15" s="1" t="inlineStr">
+        <is>
+          <t>0210-021185-106-8</t>
+        </is>
+      </c>
+      <c r="S15" s="1" t="inlineStr">
+        <is>
+          <t>0322-059358-2</t>
+        </is>
+      </c>
+      <c r="T15" s="1" t="inlineStr">
+        <is>
+          <t>MOTIVO</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>013930</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>JUAN ANTONIO  HENRIQUEZ ANZORA/SIN UNIFORME</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>0.00 </t>
+        </is>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="inlineStr">
+        <is>
+          <t>2010-02-21 00:00:00 </t>
+        </is>
+      </c>
+      <c r="G16" s="1" t="inlineStr">
+        <is>
+          <t>2010-02-21 00:00:00  </t>
+        </is>
+      </c>
+      <c r="H16" s="1" t="inlineStr">
+        <is>
+          <t>F.RETIRO</t>
+        </is>
+      </c>
+      <c r="I16" s="1" t="inlineStr">
+        <is>
+          <t>******</t>
+        </is>
+      </c>
+      <c r="J16" s="1" t="inlineStr">
+        <is>
+          <t>19/02/21</t>
+        </is>
+      </c>
+      <c r="K16" s="1" t="inlineStr">
+        <is>
+          <t>03536638-4</t>
+        </is>
+      </c>
+      <c r="L16" s="1" t="inlineStr">
+        <is>
+          <t>315301870000</t>
+        </is>
+      </c>
+      <c r="M16" s="1" t="inlineStr">
+        <is>
+          <t>0001</t>
+        </is>
+      </c>
+      <c r="N16" s="1" t="inlineStr">
+        <is>
+          <t>AGENTE DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="O16" s="1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="P16" s="1" t="inlineStr">
+        <is>
+          <t>0000-00-00</t>
+        </is>
+      </c>
+      <c r="Q16" s="1" t="inlineStr">
+        <is>
+          <t>107861358</t>
+        </is>
+      </c>
+      <c r="R16" s="1" t="inlineStr">
+        <is>
+          <t>0706-300486-101-6</t>
+        </is>
+      </c>
+      <c r="S16" s="1" t="inlineStr">
+        <is>
+          <t>0311-255798-3</t>
+        </is>
+      </c>
+      <c r="T16" s="1" t="inlineStr">
+        <is>
+          <t>MOTIVO</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>015517</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>JOSE ALBERTO  TOBAR ORTIZ/SIN UNIFORME</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>0.00 </t>
+        </is>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="F17" s="1" t="inlineStr">
+        <is>
+          <t>2006-03-23 00:00:00 </t>
+        </is>
+      </c>
+      <c r="G17" s="1" t="inlineStr">
+        <is>
+          <t>2006-03-23 00:00:00  </t>
+        </is>
+      </c>
+      <c r="H17" s="1" t="inlineStr">
+        <is>
+          <t>F.RETIRO</t>
+        </is>
+      </c>
+      <c r="I17" s="1" t="inlineStr">
+        <is>
+          <t>******</t>
+        </is>
+      </c>
+      <c r="J17" s="1" t="inlineStr">
+        <is>
+          <t>06/03/23</t>
+        </is>
+      </c>
+      <c r="K17" s="1" t="inlineStr">
+        <is>
+          <t>03879639-2</t>
+        </is>
+      </c>
+      <c r="L17" s="1" t="inlineStr">
+        <is>
+          <t>321682590002</t>
+        </is>
+      </c>
+      <c r="M17" s="1" t="inlineStr">
+        <is>
+          <t>0001</t>
+        </is>
+      </c>
+      <c r="N17" s="1" t="inlineStr">
+        <is>
+          <t>AGENTE DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="O17" s="1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="P17" s="1" t="inlineStr">
+        <is>
+          <t>0000-00-00</t>
+        </is>
+      </c>
+      <c r="Q17" s="1" t="inlineStr">
+        <is>
+          <t>107885362</t>
+        </is>
+      </c>
+      <c r="R17" s="1" t="inlineStr">
+        <is>
+          <t>0309-280188-101-0</t>
+        </is>
+      </c>
+      <c r="S17" s="1" t="inlineStr">
+        <is>
+          <t>0322-065675-1</t>
+        </is>
+      </c>
+      <c r="T17" s="1" t="inlineStr">
         <is>
           <t>MOTIVO</t>
         </is>

</xml_diff>